<commit_message>
Moved some base virtual methods into AnimatBase.cpp
Added more documentation
</commit_message>
<xml_diff>
--- a/Documentation/Doc_Conversions.xlsx
+++ b/Documentation/Doc_Conversions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Namespace</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Structure</t>
+  </si>
+  <si>
+    <t>ActivatedItem</t>
+  </si>
+  <si>
+    <t>ActivatedItemMGr</t>
   </si>
 </sst>
 </file>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,6 +443,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more comments and changed some methods to move them down into base classes
</commit_message>
<xml_diff>
--- a/Documentation/Doc_Conversions.xlsx
+++ b/Documentation/Doc_Conversions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Namespace</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>ActivatedItemMGr</t>
+  </si>
+  <si>
+    <t>organism</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,39 +421,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>